<commit_message>
Report done. (Also cleaned up other documentation.
</commit_message>
<xml_diff>
--- a/Lab 3/filter gain.xlsx
+++ b/Lab 3/filter gain.xlsx
@@ -105,6 +105,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lowpass</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> to Highpass w/ Gain=.9 @ 1kHz</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -255,12 +279,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Lo-&gt;Hi'!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
+            <c:v>3dB Down</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -336,52 +355,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.70710678118654746</c:v>
+                  <c:v>0.63639610306789274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -396,11 +415,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50264704"/>
-        <c:axId val="50263168"/>
+        <c:axId val="40112896"/>
+        <c:axId val="40114432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50264704"/>
+        <c:axId val="40112896"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -408,16 +427,35 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Freq (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50263168"/>
+        <c:crossAx val="40114432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50263168"/>
+        <c:axId val="40114432"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -425,11 +463,35 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Gain</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50264704"/>
+        <c:crossAx val="40112896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -741,11 +803,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74362880"/>
-        <c:axId val="74348800"/>
+        <c:axId val="40250368"/>
+        <c:axId val="40252160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74362880"/>
+        <c:axId val="40250368"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -757,12 +819,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74348800"/>
+        <c:crossAx val="40252160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74348800"/>
+        <c:axId val="40252160"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -774,7 +836,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74362880"/>
+        <c:crossAx val="40250368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -812,6 +874,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Bandpass filter w/ Gain=.6 @1kHz</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -992,12 +1073,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'.6'!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
+            <c:v>-3dB</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -1163,11 +1239,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="152568576"/>
-        <c:axId val="151788544"/>
+        <c:axId val="40287232"/>
+        <c:axId val="40297216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="152568576"/>
+        <c:axId val="40287232"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1175,16 +1251,35 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Freq (kHz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151788544"/>
+        <c:crossAx val="40297216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="151788544"/>
+        <c:axId val="40297216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1192,11 +1287,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltage Gain</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152568576"/>
+        <c:crossAx val="40287232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1294,12 +1408,12 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -1613,7 +1727,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,8 +1761,8 @@
         <v>0.19759277833500499</v>
       </c>
       <c r="E2">
-        <f>SQRT(2)^-1</f>
-        <v>0.70710678118654746</v>
+        <f>0.9*SQRT(2)^-1</f>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1666,8 +1780,8 @@
         <v>0.37562940584088622</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E17" si="1">SQRT(2)^-1</f>
-        <v>0.70710678118654746</v>
+        <f t="shared" ref="E3:E17" si="1">0.9*SQRT(2)^-1</f>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1686,7 +1800,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1705,7 +1819,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1724,7 +1838,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1743,7 +1857,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1762,7 +1876,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1781,7 +1895,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1800,7 +1914,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1819,7 +1933,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1838,7 +1952,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1857,7 +1971,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1876,7 +1990,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1895,7 +2009,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1914,7 +2028,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1933,7 +2047,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>0.70710678118654746</v>
+        <v>0.63639610306789274</v>
       </c>
     </row>
   </sheetData>
@@ -2280,8 +2394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>